<commit_message>
changes made to the filesa again
</commit_message>
<xml_diff>
--- a/Ex_Files_Stats_Basic/Ex_Files_Stats_Basic/Exercise Files/02_02_Exercise.xlsx
+++ b/Ex_Files_Stats_Basic/Ex_Files_Stats_Basic/Exercise Files/02_02_Exercise.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pooja\Downloads\Statistics Foundations 1- The Basics\Ex_Files_Stats_Basic\Ex_Files_Stats_Basic\Exercise Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eddiedavila/Desktop/Stats WB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1005990C-3E74-40EB-9F10-7AB125903F89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD3CEFB9-D47C-2F4A-9EBF-758E899F40AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{02E90640-9AFF-EB41-9DBB-76A9E96308E5}"/>
+    <workbookView xWindow="0" yWindow="2560" windowWidth="27420" windowHeight="15440" xr2:uid="{02E90640-9AFF-EB41-9DBB-76A9E96308E5}"/>
   </bookViews>
   <sheets>
     <sheet name="BEGIN" sheetId="5" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Data Point</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>MEAN</t>
+  </si>
+  <si>
+    <t>Average</t>
   </si>
   <si>
     <t>Most Common Value in the Data Set</t>
@@ -381,7 +384,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -399,7 +402,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -426,7 +429,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -588,7 +591,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5CA1E2AF-52A6-E541-9C31-861340359DC4}" name="Table5" displayName="Table5" ref="A1:B8" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3" totalsRowBorderDxfId="2">
   <autoFilter ref="A1:B8" xr:uid="{E0B3D01A-1402-974C-A49A-88ECF5C6E289}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B8">
-    <sortCondition ref="B1:B8"/>
+    <sortCondition ref="A1:A8"/>
   </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{D286746E-EA12-3B4F-8233-920DCD80ACB7}" name="Data Point" dataDxfId="1"/>
@@ -599,9 +602,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -639,7 +642,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -745,7 +748,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -887,7 +890,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -897,11 +900,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0708610E-8457-5F44-B8AF-F77AC55F7F39}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="19" style="1" customWidth="1"/>
     <col min="3" max="3" width="11.1640625" customWidth="1"/>
@@ -913,7 +916,7 @@
     <col min="10" max="10" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="49" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="49" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -921,7 +924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="49" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -936,7 +939,7 @@
       </c>
       <c r="F2" s="11">
         <f>(F3+1)/2</f>
-        <v>4</v>
+        <v>0.5</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>8</v>
@@ -944,159 +947,147 @@
       <c r="I2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="11">
-        <f>J3/J4</f>
-        <v>70</v>
+      <c r="J2" s="11" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="49" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="4">
-        <v>20</v>
+        <v>200</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="14">
-        <v>7</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="F3" s="14"/>
       <c r="H3" s="18"/>
       <c r="I3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="20">
-        <f>SUM(Table5[Value])</f>
-        <v>490</v>
-      </c>
+      <c r="J3" s="20"/>
     </row>
-    <row r="4" spans="1:10" ht="49" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" ht="49" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B4" s="4">
         <v>20</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="17">
-        <v>40</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F4" s="17"/>
       <c r="H4" s="21"/>
       <c r="I4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="22">
-        <v>7</v>
-      </c>
+      <c r="J4" s="22"/>
     </row>
-    <row r="5" spans="1:10" ht="49" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="4">
-        <v>40</v>
+        <v>140</v>
       </c>
       <c r="H5" s="18"/>
       <c r="I5" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="20">
+      <c r="J5" s="20" t="e">
         <f>J3/J4</f>
-        <v>70</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="49" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" ht="49" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B6" s="4">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="H6" s="15"/>
       <c r="I6" s="16"/>
       <c r="J6" s="17"/>
     </row>
-    <row r="7" spans="1:10" ht="49" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:10" ht="49" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B7" s="4">
-        <v>140</v>
+        <v>20</v>
       </c>
       <c r="D7" s="24" t="s">
         <v>2</v>
       </c>
       <c r="E7" s="25">
         <f>F4</f>
-        <v>40</v>
-      </c>
-      <c r="F7" s="26">
-        <f>F4</f>
-        <v>40</v>
+        <v>0</v>
+      </c>
+      <c r="F7" s="26" t="str">
+        <f>E4</f>
+        <v>X Value</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="49" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="49" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B8" s="8">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="D8" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="28">
+      <c r="E8" s="28" t="e">
         <f>J5</f>
-        <v>70</v>
-      </c>
-      <c r="F8" s="29">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F8" s="29" t="str">
         <f>J2</f>
-        <v>70</v>
+        <v>Average</v>
       </c>
       <c r="H8" s="9" t="s">
         <v>9</v>
       </c>
       <c r="I8" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="J8" s="11">
-        <v>20</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="J8" s="11"/>
     </row>
-    <row r="9" spans="1:10" ht="49" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" ht="49" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D9" s="30" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="31">
         <f>J8</f>
-        <v>20</v>
-      </c>
-      <c r="F9" s="32">
-        <f>J8</f>
-        <v>20</v>
+        <v>0</v>
+      </c>
+      <c r="F9" s="32" t="str">
+        <f>I8</f>
+        <v>Most Common Value in the Data Set</v>
       </c>
       <c r="H9" s="15"/>
       <c r="I9" s="16"/>
       <c r="J9" s="17"/>
     </row>
-    <row r="10" spans="1:10" ht="49" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:10" ht="49" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="12" spans="1:10" ht="49" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:10" ht="49" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:10" ht="49" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:10" ht="49" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="16" spans="1:10" ht="49" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="17" ht="49" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="18" ht="49" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="19" ht="49" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="20" ht="49" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="21" ht="49" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="22" ht="49" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="10" spans="1:10" ht="49" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:10" ht="49" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:10" ht="49" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:10" ht="49" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:10" ht="49" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:10" ht="49" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:10" ht="49" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" ht="49" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" ht="49" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" ht="49" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" ht="49" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" ht="49" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" ht="49" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>